<commit_message>
all the expoirted arcprodata ready to inport to r
</commit_message>
<xml_diff>
--- a/ProcessedData/export_to_r/gavi-trib1_XWD_export_eledata_co2.xlsx
+++ b/ProcessedData/export_to_r/gavi-trib1_XWD_export_eledata_co2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kriddie\OneDrive - University of North Carolina at Chapel Hill\Documents\Ecuador2021\ProcessedData\export_to_r\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64186F2F-2BD2-4D06-81A0-CE2DBC74177F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98EA40A-AD38-4C48-9583-7D052259EAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gavi-trib1_XWD_export_eledata_c" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>lat_fit</t>
   </si>
@@ -146,29 +146,41 @@
     <t>slope_mid</t>
   </si>
   <si>
+    <t>dist_dif_up</t>
+  </si>
+  <si>
+    <t>ele_dif_up</t>
+  </si>
+  <si>
+    <t>slope_up</t>
+  </si>
+  <si>
+    <t>catchment_pixel</t>
+  </si>
+  <si>
+    <t>underground</t>
+  </si>
+  <si>
+    <t>wetland inlet</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>point 9</t>
+  </si>
+  <si>
     <t>catchment_ha</t>
-  </si>
-  <si>
-    <t>dist_dif_up</t>
-  </si>
-  <si>
-    <t>ele_dif_up</t>
-  </si>
-  <si>
-    <t>slope_up</t>
-  </si>
-  <si>
-    <t>catchment_pixel</t>
-  </si>
-  <si>
-    <t>underground</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,8 +315,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +505,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,10 +675,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,19 +1036,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="10.875" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="18" width="10.875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="49.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="26" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" customWidth="1"/>
+    <col min="8" max="8" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.875" customWidth="1"/>
+    <col min="11" max="11" width="9.375" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="14" max="14" width="5.875" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="18" max="18" width="10.75" customWidth="1"/>
+    <col min="19" max="19" width="7.125" customWidth="1"/>
+    <col min="20" max="20" width="49.25" customWidth="1"/>
+    <col min="21" max="27" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -1036,76 +1074,76 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>34</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>35</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>36</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>39</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>37</v>
       </c>
       <c r="AB1" t="s">
         <v>19</v>
@@ -1124,26 +1162,23 @@
       <c r="C2">
         <v>4101.0863259999996</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2">
         <v>1.675</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>11095.728999999999</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>7.22</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>626.95140000000004</v>
-      </c>
-      <c r="AA2">
-        <v>0.52649999999999997</v>
       </c>
       <c r="AB2">
         <v>3.9999999999999998E-6</v>
@@ -1162,26 +1197,23 @@
       <c r="C3">
         <v>4101.0863259999996</v>
       </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
       <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2">
         <v>1.26</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>5319.1662429999997</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>7.2240000000000002</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>626.82839999999999</v>
-      </c>
-      <c r="AA3">
-        <v>0.53910000000000002</v>
       </c>
       <c r="AB3">
         <v>3.9999999999999998E-6</v>
@@ -1200,56 +1232,57 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
-        <v>4092.6591796875</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="3">
         <v>1130</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4*3*3*0.0001</f>
+        <v>1.0170000000000001</v>
       </c>
       <c r="F4">
         <v>37.118686429999997</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
+        <v>4092.6591796875</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>44</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>44376</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>3.0049999999999999</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>11098.654</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
       </c>
       <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="O4">
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4">
         <v>7.2320000000000002</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>626.75639999999999</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>22</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>23</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>24</v>
-      </c>
-      <c r="AA4">
-        <v>0.9486</v>
       </c>
       <c r="AB4">
         <v>3.9999999999999998E-6</v>
@@ -1269,46 +1302,47 @@
         <v>21</v>
       </c>
       <c r="D5">
-        <v>4091.66357421875</v>
-      </c>
-      <c r="E5">
         <v>1146</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E34" si="0">D5*3*3*0.0001</f>
+        <v>1.0314000000000001</v>
       </c>
       <c r="F5">
         <v>53.54342098</v>
       </c>
-      <c r="J5" s="1">
+      <c r="G5">
+        <v>4091.66357421875</v>
+      </c>
+      <c r="K5" s="1">
         <v>44376</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.20499999999999999</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>7979.2669130000004</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>4.9610000000000003</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.18870000000000001</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>7.2389999999999999</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>626.79639999999995</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>23</v>
       </c>
-      <c r="S5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA5">
-        <v>1.0268999999999999</v>
+      <c r="T5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1322,46 +1356,47 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <v>4089.491455078125</v>
-      </c>
-      <c r="E6">
         <v>1239</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1151</v>
       </c>
       <c r="F6">
         <v>68.897829580000007</v>
       </c>
-      <c r="J6" s="1">
+      <c r="G6">
+        <v>4089.491455078125</v>
+      </c>
+      <c r="K6" s="1">
         <v>44376</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>11206.38178</v>
-      </c>
-      <c r="M6" t="s">
-        <v>21</v>
       </c>
       <c r="N6" t="s">
         <v>21</v>
       </c>
-      <c r="O6">
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6">
         <v>7.2439999999999998</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>626.7364</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>22</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>23</v>
       </c>
-      <c r="S6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA6">
-        <v>1.1304000000000001</v>
+      <c r="T6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -1374,53 +1409,57 @@
       <c r="C7">
         <v>4091.229366</v>
       </c>
-      <c r="D7">
-        <v>4091.66357421875</v>
-      </c>
-      <c r="E7">
-        <v>1146</v>
+      <c r="D7" s="3">
+        <v>1256</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1304000000000001</v>
       </c>
       <c r="F7">
         <v>70.662581329999995</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
+        <v>4089.04833984375</v>
+      </c>
+      <c r="H7">
         <v>22</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>7</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>25</v>
       </c>
-      <c r="T7">
-        <v>20</v>
-      </c>
-      <c r="U7" t="e">
-        <f>F8-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V7" t="e">
-        <f>D8-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W7" t="e">
-        <f>ABS(V7)/U7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X7" t="e">
-        <f>F7-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Y7" t="e">
-        <f>D7-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Z7" t="e">
-        <f>ABS(Y7)/X7</f>
-        <v>#REF!</v>
+      <c r="U7">
+        <v>10</v>
+      </c>
+      <c r="V7">
+        <f>F9-F6</f>
+        <v>16.059034519999997</v>
+      </c>
+      <c r="W7">
+        <f>G9-G6</f>
+        <v>-1.07080078125</v>
+      </c>
+      <c r="X7">
+        <f>ABS(W7)/V7</f>
+        <v>6.6679026059531771E-2</v>
+      </c>
+      <c r="Y7">
+        <f>F7-F5</f>
+        <v>17.119160349999994</v>
+      </c>
+      <c r="Z7">
+        <f>G7-G5</f>
+        <v>-2.615234375</v>
+      </c>
+      <c r="AA7">
+        <f>ABS(Z7)/Y7</f>
+        <v>0.15276650966120547</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -1433,50 +1472,54 @@
       <c r="C8">
         <v>4089.812316</v>
       </c>
-      <c r="D8">
-        <v>4089.04833984375</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="3">
         <v>1256</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1304000000000001</v>
       </c>
       <c r="F8">
         <v>77.973254580000003</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
+        <v>4089.04833984375</v>
+      </c>
+      <c r="H8">
         <v>30</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>35</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>10</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <f>F10-F7</f>
         <v>16.449014810000008</v>
       </c>
-      <c r="V8">
-        <f>D10-D7</f>
-        <v>-4.459716796875</v>
-      </c>
       <c r="W8">
-        <f t="shared" ref="W8:W32" si="0">ABS(V8)/U8</f>
-        <v>0.27112364165200709</v>
+        <f>G10-G7</f>
+        <v>-1.844482421875</v>
       </c>
       <c r="X8">
-        <f>F8-F7</f>
-        <v>7.3106732500000078</v>
+        <f t="shared" ref="X8:X34" si="1">ABS(W8)/V8</f>
+        <v>0.11213330665576798</v>
       </c>
       <c r="Y8">
-        <f>D8-D7</f>
+        <f>F8-F5</f>
+        <v>24.429833600000002</v>
+      </c>
+      <c r="Z8">
+        <f>G8-G5</f>
         <v>-2.615234375</v>
       </c>
-      <c r="Z8">
-        <f>ABS(Y8)/X8</f>
-        <v>0.3577282536871686</v>
+      <c r="AA8">
+        <f>ABS(Z8)/Y8</f>
+        <v>0.10705084683835095</v>
       </c>
       <c r="AB8">
         <v>3.9999999999999998E-6</v>
@@ -1493,43 +1536,44 @@
         <v>21</v>
       </c>
       <c r="D9">
-        <v>4088.420654296875</v>
-      </c>
-      <c r="E9">
         <v>1318</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1862000000000001</v>
       </c>
       <c r="F9">
         <v>84.956864100000004</v>
       </c>
-      <c r="J9" s="1">
+      <c r="G9">
+        <v>4088.420654296875</v>
+      </c>
+      <c r="K9" s="1">
         <v>44376</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.34499999999999997</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>3489.7833529999998</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>4.5579999999999998</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.1381</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>7.2489999999999997</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>626.76340000000005</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>22</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>23</v>
-      </c>
-      <c r="AA9">
-        <v>1.1934</v>
       </c>
       <c r="AC9">
         <v>8.9507499999999993</v>
@@ -1545,53 +1589,57 @@
       <c r="C10">
         <v>4087.4567360000001</v>
       </c>
-      <c r="D10">
-        <v>4087.203857421875</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="3">
         <v>1337</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2033</v>
       </c>
       <c r="F10">
         <v>87.111596140000003</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
+        <v>4087.203857421875</v>
+      </c>
+      <c r="H10">
         <v>40</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>7</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>33</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>26</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>10</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <f>F11-F8</f>
         <v>18.988651259999997</v>
       </c>
-      <c r="V10">
-        <f>D11-D8</f>
-        <v>0</v>
-      </c>
       <c r="W10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G11-G8</f>
+        <v>-2.959716796875</v>
       </c>
       <c r="X10">
+        <f t="shared" si="1"/>
+        <v>0.15586766834302271</v>
+      </c>
+      <c r="Y10">
         <f>F10-F7</f>
         <v>16.449014810000008</v>
       </c>
-      <c r="Y10">
-        <f>D10-D7</f>
-        <v>-4.459716796875</v>
-      </c>
       <c r="Z10">
-        <f>ABS(Y10)/X10</f>
-        <v>0.27112364165200709</v>
+        <f>G10-G7</f>
+        <v>-1.844482421875</v>
+      </c>
+      <c r="AA10">
+        <f>ABS(Z10)/Y10</f>
+        <v>0.11213330665576798</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -1604,50 +1652,54 @@
       <c r="C11">
         <v>4083.8392039999999</v>
       </c>
-      <c r="D11">
-        <v>4089.04833984375</v>
-      </c>
-      <c r="E11">
-        <v>1256</v>
+      <c r="D11" s="3">
+        <v>1358</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2222</v>
       </c>
       <c r="F11">
         <v>96.96190584</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
+        <v>4086.088623046875</v>
+      </c>
+      <c r="H11">
         <v>50</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>7.5</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>15</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>10</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <f>F13-F10</f>
         <v>16.752185659999995</v>
       </c>
-      <c r="V11">
-        <f>D13-D10</f>
-        <v>-2.6440434218748123</v>
-      </c>
       <c r="W11">
-        <f t="shared" si="0"/>
-        <v>0.15783274347228152</v>
+        <f>G13-G10</f>
+        <v>-2.873046875</v>
       </c>
       <c r="X11">
+        <f t="shared" si="1"/>
+        <v>0.17150280765214496</v>
+      </c>
+      <c r="Y11">
         <f>F11-F8</f>
         <v>18.988651259999997</v>
       </c>
-      <c r="Y11">
-        <f>D11-D8</f>
-        <v>0</v>
-      </c>
       <c r="Z11">
-        <f>ABS(Y11)/X11</f>
-        <v>0</v>
+        <f>G11-G8</f>
+        <v>-2.959716796875</v>
+      </c>
+      <c r="AA11">
+        <f>ABS(Z11)/Y11</f>
+        <v>0.15586766834302271</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -1660,38 +1712,45 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
+      <c r="D12">
+        <v>1360</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.224</v>
+      </c>
       <c r="F12">
         <v>102.69983089999999</v>
       </c>
-      <c r="J12" s="1">
+      <c r="G12">
+        <v>4084.92919921875</v>
+      </c>
+      <c r="K12" s="1">
         <v>44370</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.93</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1895.8114720000001</v>
-      </c>
-      <c r="M12" t="s">
-        <v>21</v>
       </c>
       <c r="N12" t="s">
         <v>21</v>
       </c>
-      <c r="O12">
+      <c r="O12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12">
         <v>6.7510000000000003</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>627.7894</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>27</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>23</v>
-      </c>
-      <c r="AA12">
-        <v>1.2231000000000001</v>
       </c>
       <c r="AC12">
         <v>8.4662500000000005</v>
@@ -1707,22 +1766,29 @@
       <c r="C13">
         <v>4081.9244720000002</v>
       </c>
-      <c r="D13">
-        <v>4084.5598140000002</v>
+      <c r="D13" s="3">
+        <v>1361</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2249000000000001</v>
       </c>
       <c r="F13">
         <v>103.8637818</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
+        <v>4084.330810546875</v>
+      </c>
+      <c r="H13">
         <v>58</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>18</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1736,47 +1802,54 @@
       <c r="C14">
         <v>4080.4015720000002</v>
       </c>
-      <c r="D14">
-        <v>4082.695557</v>
+      <c r="D14" s="3">
+        <v>1363</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2267000000000001</v>
       </c>
       <c r="F14">
         <v>115.1746814</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
+        <v>4083.16455078125</v>
+      </c>
+      <c r="H14">
         <v>70</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>80</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>20</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <f>F16-F13</f>
         <v>20.890311300000008</v>
       </c>
-      <c r="V14">
-        <f>D16-D13</f>
-        <v>-3.7333980000003066</v>
-      </c>
       <c r="W14">
-        <f t="shared" si="0"/>
-        <v>0.17871433059976974</v>
+        <f>G16-G13</f>
+        <v>-2.875244140625</v>
       </c>
       <c r="X14">
+        <f t="shared" si="1"/>
+        <v>0.13763529414829731</v>
+      </c>
+      <c r="Y14">
         <f>F14-F11</f>
         <v>18.212775559999997</v>
       </c>
-      <c r="Y14">
-        <f>D14-D11</f>
-        <v>-6.352782843749992</v>
-      </c>
       <c r="Z14">
-        <f>ABS(Y14)/X14</f>
-        <v>0.34880915447628746</v>
+        <f>G14-G11</f>
+        <v>-2.924072265625</v>
+      </c>
+      <c r="AA14">
+        <f>ABS(Z14)/Y14</f>
+        <v>0.16055061217835601</v>
       </c>
       <c r="AB14">
         <v>9.8999999999999994E-5</v>
@@ -1792,38 +1865,45 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
+      <c r="D15">
+        <v>1365</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2285000000000001</v>
+      </c>
       <c r="F15">
         <v>121.68240230000001</v>
       </c>
-      <c r="J15" s="1">
+      <c r="G15">
+        <v>4082.015869140625</v>
+      </c>
+      <c r="K15" s="1">
         <v>44370</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1.0149999999999999</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>4538.9951879999999</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>3.6509999999999998</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.2276</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>6.7530000000000001</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>627.62339999999995</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>27</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>23</v>
-      </c>
-      <c r="AA15">
-        <v>1.2284999999999999</v>
       </c>
       <c r="AC15">
         <v>8.6712500000000006</v>
@@ -1839,50 +1919,57 @@
       <c r="C16">
         <v>4080.0840429999998</v>
       </c>
-      <c r="D16">
-        <v>4080.8264159999999</v>
+      <c r="D16" s="3">
+        <v>1366</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2294</v>
       </c>
       <c r="F16">
         <v>124.75409310000001</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
+        <v>4081.45556640625</v>
+      </c>
+      <c r="H16">
         <v>80</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.5</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>28</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>29</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>10</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <f>F17-F14</f>
         <v>19.725041000000004</v>
       </c>
-      <c r="V16">
-        <f>D17-D14</f>
-        <v>-3.4401859999998123</v>
-      </c>
       <c r="W16">
-        <f>ABS(V16)/U16</f>
-        <v>0.17440703925532078</v>
+        <f>G17-G14</f>
+        <v>-3.2939453125</v>
       </c>
       <c r="X16">
+        <f>ABS(W16)/V16</f>
+        <v>0.16699307811324698</v>
+      </c>
+      <c r="Y16">
         <f>F16-F13</f>
         <v>20.890311300000008</v>
       </c>
-      <c r="Y16">
-        <f>D16-D13</f>
-        <v>-3.7333980000003066</v>
-      </c>
       <c r="Z16">
-        <f>ABS(Y16)/X16</f>
-        <v>0.17871433059976974</v>
+        <f>G16-G13</f>
+        <v>-2.875244140625</v>
+      </c>
+      <c r="AA16">
+        <f>ABS(Z16)/Y16</f>
+        <v>0.13763529414829731</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
@@ -1895,50 +1982,57 @@
       <c r="C17">
         <v>4079.6831520000001</v>
       </c>
-      <c r="D17">
-        <v>4079.2553710000002</v>
+      <c r="D17" s="3">
+        <v>1369</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2321</v>
       </c>
       <c r="F17">
         <v>134.8997224</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
+        <v>4079.87060546875</v>
+      </c>
+      <c r="H17">
         <v>90</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.5</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>23</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>29</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>10</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <f>F19-F16</f>
         <v>21.253888099999983</v>
       </c>
-      <c r="V17">
-        <f>D19-D16</f>
-        <v>-3.195067999999992</v>
-      </c>
       <c r="W17">
-        <f t="shared" si="0"/>
-        <v>0.15032863563443691</v>
+        <f>G19-G16</f>
+        <v>-3.291748046875</v>
       </c>
       <c r="X17">
+        <f t="shared" si="1"/>
+        <v>0.15487745260477789</v>
+      </c>
+      <c r="Y17">
         <f>F17-F14</f>
         <v>19.725041000000004</v>
       </c>
-      <c r="Y17">
-        <f>D17-D14</f>
-        <v>-3.4401859999998123</v>
-      </c>
       <c r="Z17">
-        <f>ABS(Y17)/X17</f>
-        <v>0.17440703925532078</v>
+        <f>G17-G14</f>
+        <v>-3.2939453125</v>
+      </c>
+      <c r="AA17">
+        <f>ABS(Z17)/Y17</f>
+        <v>0.16699307811324698</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
@@ -1951,38 +2045,45 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
+      <c r="D18">
+        <v>1370</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2330000000000001</v>
+      </c>
       <c r="F18">
         <v>135.01395909999999</v>
       </c>
-      <c r="J18" s="1">
+      <c r="G18">
+        <v>4079.38232421875</v>
+      </c>
+      <c r="K18" s="1">
         <v>44370</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>0.58499999999999996</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>1924.7162740000001</v>
-      </c>
-      <c r="M18" t="s">
-        <v>21</v>
       </c>
       <c r="N18" t="s">
         <v>21</v>
       </c>
-      <c r="O18">
+      <c r="O18" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18">
         <v>6.7539999999999996</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>627.74739999999997</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>27</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>23</v>
-      </c>
-      <c r="AA18">
-        <v>1.2330000000000001</v>
       </c>
       <c r="AC18">
         <v>8.7735000000000003</v>
@@ -1998,50 +2099,57 @@
       <c r="C19">
         <v>4078.8270910000001</v>
       </c>
-      <c r="D19">
-        <v>4077.6313479999999</v>
+      <c r="D19" s="3">
+        <v>1373</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2357</v>
       </c>
       <c r="F19">
         <v>146.00798119999999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
+        <v>4078.163818359375</v>
+      </c>
+      <c r="H19">
         <v>100</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>1.5</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>14</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>30</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>10</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <f>F20-F17</f>
         <v>20.73320480000001</v>
       </c>
-      <c r="V19">
-        <f>D20-D17</f>
-        <v>-2.456543000000238</v>
-      </c>
       <c r="W19">
-        <f t="shared" si="0"/>
-        <v>0.11848351587209696</v>
+        <f>G20-G17</f>
+        <v>-2.998046875</v>
       </c>
       <c r="X19">
+        <f t="shared" si="1"/>
+        <v>0.14460122802626243</v>
+      </c>
+      <c r="Y19">
         <f>F19-F16</f>
         <v>21.253888099999983</v>
       </c>
-      <c r="Y19">
-        <f>D19-D16</f>
-        <v>-3.195067999999992</v>
-      </c>
       <c r="Z19">
-        <f>ABS(Y19)/X19</f>
-        <v>0.15032863563443691</v>
+        <f>G19-G16</f>
+        <v>-3.291748046875</v>
+      </c>
+      <c r="AA19">
+        <f>ABS(Z19)/Y19</f>
+        <v>0.15487745260477789</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -2054,47 +2162,54 @@
       <c r="C20">
         <v>4077.7807090000001</v>
       </c>
-      <c r="D20">
-        <v>4076.798828</v>
+      <c r="D20" s="3">
+        <v>1405</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2645</v>
       </c>
       <c r="F20">
         <v>155.63292720000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
+        <v>4076.87255859375</v>
+      </c>
+      <c r="H20">
         <v>110</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>2</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>9</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>10</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <f>F22-F19</f>
         <v>19.976151700000003</v>
       </c>
-      <c r="V20">
-        <f>D22-D19</f>
-        <v>-1.3300779999999577</v>
-      </c>
       <c r="W20">
-        <f t="shared" si="0"/>
-        <v>6.6583294919609445E-2</v>
+        <f>G22-G19</f>
+        <v>-1.89794921875</v>
       </c>
       <c r="X20">
+        <f t="shared" si="1"/>
+        <v>9.5010753184758795E-2</v>
+      </c>
+      <c r="Y20">
         <f>F20-F17</f>
         <v>20.73320480000001</v>
       </c>
-      <c r="Y20">
-        <f>D20-D17</f>
-        <v>-2.456543000000238</v>
-      </c>
       <c r="Z20">
-        <f>ABS(Y20)/X20</f>
-        <v>0.11848351587209696</v>
+        <f>G20-G17</f>
+        <v>-2.998046875</v>
+      </c>
+      <c r="AA20">
+        <f>ABS(Z20)/Y20</f>
+        <v>0.14460122802626243</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -2107,38 +2222,45 @@
       <c r="C21" t="s">
         <v>21</v>
       </c>
+      <c r="D21">
+        <v>1406</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2654000000000001</v>
+      </c>
       <c r="F21">
         <v>159.9350599</v>
       </c>
-      <c r="J21" s="1">
+      <c r="G21">
+        <v>4076.6494140625</v>
+      </c>
+      <c r="K21" s="1">
         <v>44370</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>0.82</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>2613.9688449999999</v>
-      </c>
-      <c r="M21" t="s">
-        <v>21</v>
       </c>
       <c r="N21" t="s">
         <v>21</v>
       </c>
-      <c r="O21">
+      <c r="O21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21">
         <v>6.7539999999999996</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>627.65639999999996</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>27</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>23</v>
-      </c>
-      <c r="AA21">
-        <v>1.2663</v>
       </c>
       <c r="AC21">
         <v>8.9039999999999999</v>
@@ -2154,47 +2276,54 @@
       <c r="C22">
         <v>4076.911893</v>
       </c>
-      <c r="D22">
-        <v>4076.3012699999999</v>
+      <c r="D22" s="3">
+        <v>1408</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2672000000000001</v>
       </c>
       <c r="F22">
         <v>165.98413289999999</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
+        <v>4076.265869140625</v>
+      </c>
+      <c r="H22">
         <v>120</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>5.5</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>15</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>10</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <f>F23-F20</f>
         <v>21.013665500000002</v>
       </c>
-      <c r="V22">
-        <f>D23-D20</f>
-        <v>-0.97607400000015332</v>
-      </c>
       <c r="W22">
-        <f t="shared" si="0"/>
-        <v>4.6449487834483383E-2</v>
+        <f>G23-G20</f>
+        <v>-0.9697265625</v>
       </c>
       <c r="X22">
+        <f t="shared" si="1"/>
+        <v>4.614742546939276E-2</v>
+      </c>
+      <c r="Y22">
         <f>F22-F19</f>
         <v>19.976151700000003</v>
       </c>
-      <c r="Y22">
-        <f>D22-D19</f>
-        <v>-1.3300779999999577</v>
-      </c>
       <c r="Z22">
-        <f>ABS(Y22)/X22</f>
-        <v>6.6583294919609445E-2</v>
+        <f>G22-G19</f>
+        <v>-1.89794921875</v>
+      </c>
+      <c r="AA22">
+        <f>ABS(Z22)/Y22</f>
+        <v>9.5010753184758795E-2</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
@@ -2207,47 +2336,54 @@
       <c r="C23">
         <v>4076.2066279999999</v>
       </c>
-      <c r="D23">
-        <v>4075.8227539999998</v>
+      <c r="D23" s="3">
+        <v>1410</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2690000000000001</v>
       </c>
       <c r="F23">
         <v>176.64659270000001</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
+        <v>4075.90283203125</v>
+      </c>
+      <c r="H23">
         <v>130</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>2</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>13</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>10</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <f>F25-F22</f>
         <v>20.1363317</v>
       </c>
-      <c r="V23">
-        <f>D25-D22</f>
-        <v>-0.96533199999976205</v>
-      </c>
       <c r="W23">
-        <f t="shared" si="0"/>
-        <v>4.7939814181734104E-2</v>
+        <f>G25-G22</f>
+        <v>-0.929931640625</v>
       </c>
       <c r="X23">
+        <f t="shared" si="1"/>
+        <v>4.6181780002412257E-2</v>
+      </c>
+      <c r="Y23">
         <f>F23-F20</f>
         <v>21.013665500000002</v>
       </c>
-      <c r="Y23">
-        <f>D23-D20</f>
-        <v>-0.97607400000015332</v>
-      </c>
       <c r="Z23">
-        <f>ABS(Y23)/X23</f>
-        <v>4.6449487834483383E-2</v>
+        <f>G23-G20</f>
+        <v>-0.9697265625</v>
+      </c>
+      <c r="AA23">
+        <f>ABS(Z23)/Y23</f>
+        <v>4.614742546939276E-2</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
@@ -2260,38 +2396,45 @@
       <c r="C24" t="s">
         <v>21</v>
       </c>
+      <c r="D24">
+        <v>1412</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2708000000000002</v>
+      </c>
       <c r="F24">
         <v>182.55125839999999</v>
       </c>
-      <c r="J24" s="1">
+      <c r="G24">
+        <v>4075.5234375</v>
+      </c>
+      <c r="K24" s="1">
         <v>44370</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1.34</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>2415.4169040000002</v>
-      </c>
-      <c r="M24" t="s">
-        <v>21</v>
       </c>
       <c r="N24" t="s">
         <v>21</v>
       </c>
-      <c r="O24">
+      <c r="O24" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24">
         <v>6.7549999999999999</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>627.50040000000001</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>27</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>23</v>
-      </c>
-      <c r="AA24">
-        <v>1.2707999999999999</v>
       </c>
       <c r="AC24">
         <v>9.2260000000000009</v>
@@ -2307,460 +2450,580 @@
       <c r="C25">
         <v>4075.7494620000002</v>
       </c>
-      <c r="D25">
-        <v>4075.3359380000002</v>
+      <c r="D25" s="3">
+        <v>1413</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2717000000000001</v>
       </c>
       <c r="F25">
         <v>186.12046459999999</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
+        <v>4075.3359375</v>
+      </c>
+      <c r="H25">
         <v>140</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>1.5</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>33</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>10</v>
       </c>
-      <c r="U25">
-        <f>F26-F23</f>
+      <c r="V25">
+        <f>F27-F23</f>
         <v>17.638401699999974</v>
       </c>
-      <c r="V25">
-        <f>D26-D23</f>
-        <v>-0.83618200000000797</v>
-      </c>
       <c r="W25">
-        <f t="shared" si="0"/>
-        <v>4.7406903086916835E-2</v>
+        <f>G27-G23</f>
+        <v>-0.916259765625</v>
       </c>
       <c r="X25">
+        <f t="shared" si="1"/>
+        <v>5.1946870312234772E-2</v>
+      </c>
+      <c r="Y25">
         <f>F25-F22</f>
         <v>20.1363317</v>
       </c>
-      <c r="Y25">
-        <f>D25-D22</f>
-        <v>-0.96533199999976205</v>
-      </c>
       <c r="Z25">
-        <f>ABS(Y25)/X25</f>
-        <v>4.7939814181734104E-2</v>
+        <f>G25-G22</f>
+        <v>-0.929931640625</v>
+      </c>
+      <c r="AA25">
+        <f>ABS(Z25)/Y25</f>
+        <v>4.6181780002412257E-2</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>-0.33005391299999998</v>
-      </c>
-      <c r="B26">
-        <v>-78.202099230000002</v>
-      </c>
-      <c r="C26">
-        <v>4075.5669280000002</v>
-      </c>
       <c r="D26">
-        <v>4074.9865719999998</v>
-      </c>
-      <c r="F26">
-        <v>194.28499439999999</v>
+        <v>1414</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2726</v>
       </c>
       <c r="G26">
-        <v>150</v>
-      </c>
-      <c r="H26">
-        <v>11</v>
-      </c>
-      <c r="I26">
-        <v>20</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26">
-        <f>F27-F25</f>
-        <v>19.135126299999996</v>
-      </c>
-      <c r="V26">
-        <f>D27-D25</f>
-        <v>-0.77417000000014013</v>
-      </c>
-      <c r="W26">
-        <f t="shared" si="0"/>
-        <v>4.045805540359252E-2</v>
-      </c>
-      <c r="X26">
-        <f>F26-F23</f>
-        <v>17.638401699999974</v>
-      </c>
-      <c r="Y26">
-        <f>D26-D23</f>
-        <v>-0.83618200000000797</v>
-      </c>
-      <c r="Z26">
-        <f>ABS(Y26)/X26</f>
-        <v>4.7406903086916835E-2</v>
+        <v>4075.160888671875</v>
+      </c>
+      <c r="I26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>44</v>
+      </c>
+      <c r="T26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>-0.33013471300000002</v>
+        <v>-0.33005391299999998</v>
       </c>
       <c r="B27">
-        <v>-78.202155419999997</v>
+        <v>-78.202099230000002</v>
       </c>
       <c r="C27">
-        <v>4075.296738</v>
-      </c>
-      <c r="D27">
-        <v>4074.561768</v>
+        <v>4075.5669280000002</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1415</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2735000000000001</v>
       </c>
       <c r="F27">
-        <v>205.25559089999999</v>
-      </c>
-      <c r="G27">
-        <v>160</v>
+        <v>194.28499439999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4074.986572265625</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="I27">
-        <v>26</v>
-      </c>
-      <c r="S27" t="s">
-        <v>31</v>
-      </c>
-      <c r="T27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>20</v>
+      </c>
+      <c r="U27">
         <v>10</v>
       </c>
-      <c r="U27">
-        <f>F29-F26</f>
-        <v>20.940894800000024</v>
-      </c>
       <c r="V27">
-        <f>D29-D26</f>
-        <v>-0.74853499999971973</v>
+        <f>F28-F25</f>
+        <v>19.135126299999996</v>
       </c>
       <c r="W27">
-        <f t="shared" si="0"/>
-        <v>3.5745129668466644E-2</v>
+        <f>G28-G25</f>
+        <v>-0.8310546875</v>
       </c>
       <c r="X27">
-        <f>F27-F25</f>
-        <v>19.135126299999996</v>
+        <f t="shared" si="1"/>
+        <v>4.3430844117292297E-2</v>
       </c>
       <c r="Y27">
-        <f>D27-D25</f>
-        <v>-0.77417000000014013</v>
+        <f>F27-F23</f>
+        <v>17.638401699999974</v>
       </c>
       <c r="Z27">
-        <f>ABS(Y27)/X27</f>
-        <v>4.045805540359252E-2</v>
+        <f>G27-G23</f>
+        <v>-0.916259765625</v>
+      </c>
+      <c r="AA27">
+        <f>ABS(Z27)/Y27</f>
+        <v>5.1946870312234772E-2</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-0.33017421299999999</v>
+        <v>-0.33013471300000002</v>
       </c>
       <c r="B28">
-        <v>-78.202173880000004</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
+        <v>-78.202155419999997</v>
+      </c>
+      <c r="C28">
+        <v>4075.296738</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1418</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2762</v>
       </c>
       <c r="F28">
-        <v>210.11278709999999</v>
-      </c>
-      <c r="J28" s="1">
-        <v>44370</v>
-      </c>
-      <c r="K28">
-        <v>0.68</v>
-      </c>
-      <c r="L28">
-        <v>2334.2532940000001</v>
-      </c>
-      <c r="M28" t="s">
-        <v>21</v>
-      </c>
-      <c r="N28" t="s">
-        <v>21</v>
-      </c>
-      <c r="O28">
-        <v>6.7539999999999996</v>
-      </c>
-      <c r="P28">
-        <v>627.34439999999995</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>27</v>
-      </c>
-      <c r="R28" t="s">
-        <v>23</v>
+        <v>205.25559089999999</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4074.5048828125</v>
+      </c>
+      <c r="H28">
+        <v>160</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>26</v>
+      </c>
+      <c r="T28" t="s">
+        <v>31</v>
+      </c>
+      <c r="U28">
+        <v>10</v>
+      </c>
+      <c r="V28">
+        <f>F30-F27</f>
+        <v>20.940894800000024</v>
+      </c>
+      <c r="W28">
+        <f>G30-G27</f>
+        <v>-0.829833984375</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="1"/>
+        <v>3.9627436759531356E-2</v>
+      </c>
+      <c r="Y28">
+        <f>F28-F25</f>
+        <v>19.135126299999996</v>
+      </c>
+      <c r="Z28">
+        <f>G28-G25</f>
+        <v>-0.8310546875</v>
       </c>
       <c r="AA28">
-        <v>1.2770999999999999</v>
-      </c>
-      <c r="AC28">
-        <v>9.3874999999999993</v>
+        <f>ABS(Z28)/Y28</f>
+        <v>4.3430844117292297E-2</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>-0.33021831299999999</v>
+        <v>-0.33017421299999999</v>
       </c>
       <c r="B29">
-        <v>-78.202186699999999</v>
-      </c>
-      <c r="C29">
-        <v>4074.8034990000001</v>
+        <v>-78.202173880000004</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
       </c>
       <c r="D29">
-        <v>4074.2380370000001</v>
+        <v>1419</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2771000000000001</v>
       </c>
       <c r="F29">
-        <v>215.22588920000001</v>
+        <v>210.11278709999999</v>
       </c>
       <c r="G29">
-        <v>170</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29">
-        <v>46</v>
-      </c>
-      <c r="T29">
-        <v>10</v>
-      </c>
-      <c r="U29">
-        <f>F30-F27</f>
-        <v>19.940596600000021</v>
-      </c>
-      <c r="V29">
-        <f>D30-D27</f>
-        <v>-0.59155300000020361</v>
-      </c>
-      <c r="W29">
-        <f t="shared" si="0"/>
-        <v>2.9665762357391202E-2</v>
-      </c>
-      <c r="X29">
-        <f>F29-F26</f>
-        <v>20.940894800000024</v>
-      </c>
-      <c r="Y29">
-        <f>D29-D26</f>
-        <v>-0.74853499999971973</v>
-      </c>
-      <c r="Z29">
-        <f>ABS(Y29)/X29</f>
-        <v>3.5745129668466644E-2</v>
+        <v>4074.365966796875</v>
+      </c>
+      <c r="K29" s="1">
+        <v>44370</v>
+      </c>
+      <c r="L29">
+        <v>0.68</v>
+      </c>
+      <c r="M29">
+        <v>2334.2532940000001</v>
+      </c>
+      <c r="N29" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" t="s">
+        <v>21</v>
+      </c>
+      <c r="P29">
+        <v>6.7539999999999996</v>
+      </c>
+      <c r="Q29">
+        <v>627.34439999999995</v>
+      </c>
+      <c r="R29" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC29">
+        <v>9.3874999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>-0.33030731299999999</v>
+        <v>-0.33021831299999999</v>
       </c>
       <c r="B30">
-        <v>-78.202195029999999</v>
+        <v>-78.202186699999999</v>
       </c>
       <c r="C30">
-        <v>4074.1683619999999</v>
+        <v>4074.8034990000001</v>
       </c>
       <c r="D30">
-        <v>4073.9702149999998</v>
+        <v>1600</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4400000000000002</v>
       </c>
       <c r="F30">
-        <v>225.19618750000001</v>
+        <v>215.22588920000001</v>
       </c>
       <c r="G30">
-        <v>180</v>
+        <v>4074.15673828125</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="I30">
-        <v>144</v>
-      </c>
-      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>46</v>
+      </c>
+      <c r="U30">
         <v>10</v>
       </c>
-      <c r="U30">
-        <f>F31-F29</f>
-        <v>19.940596599999992</v>
-      </c>
       <c r="V30">
-        <f>D31-D29</f>
-        <v>-0.77514599999994971</v>
+        <f>F32-F28</f>
+        <v>19.940596600000021</v>
       </c>
       <c r="W30">
-        <f t="shared" si="0"/>
-        <v>3.8872758701710558E-2</v>
+        <f>G32-G28</f>
+        <v>-0.601318359375</v>
       </c>
       <c r="X30">
+        <f t="shared" si="1"/>
+        <v>3.0155484885291715E-2</v>
+      </c>
+      <c r="Y30">
         <f>F30-F27</f>
-        <v>19.940596600000021</v>
-      </c>
-      <c r="Y30">
-        <f>D30-D27</f>
-        <v>-0.59155300000020361</v>
+        <v>20.940894800000024</v>
       </c>
       <c r="Z30">
-        <f>ABS(Y30)/X30</f>
-        <v>2.9665762357391202E-2</v>
-      </c>
-      <c r="AB30">
-        <v>2.4800000000000001E-4</v>
+        <f>G30-G27</f>
+        <v>-0.829833984375</v>
+      </c>
+      <c r="AA30">
+        <f>ABS(Z30)/Y30</f>
+        <v>3.9627436759531356E-2</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>-0.33039551299999997</v>
+        <v>-0.33025371307349199</v>
       </c>
       <c r="B31">
-        <v>-78.202208720000002</v>
+        <v>-78.202191908147697</v>
       </c>
       <c r="C31">
-        <v>4073.2208500000002</v>
+        <v>4074.56262131828</v>
       </c>
       <c r="D31">
-        <v>4073.4628910000001</v>
+        <v>1656</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4904000000000002</v>
       </c>
       <c r="F31">
-        <v>235.1664858</v>
+        <f>F32-3.9881193192405</f>
+        <v>221.20806818075951</v>
       </c>
       <c r="G31">
-        <v>190</v>
+        <v>4074.076416015625</v>
       </c>
       <c r="H31">
-        <v>5.5</v>
-      </c>
-      <c r="I31">
-        <v>40</v>
-      </c>
-      <c r="S31" t="s">
-        <v>32</v>
-      </c>
-      <c r="T31">
-        <v>10</v>
-      </c>
-      <c r="U31">
-        <f t="shared" ref="U31" si="1">F32-F30</f>
-        <v>19.475454899999988</v>
-      </c>
-      <c r="V31">
-        <f>D32-D30</f>
-        <v>-0.82299799999964307</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="0"/>
-        <v>4.2258217033977655E-2</v>
-      </c>
-      <c r="X31">
-        <f>F31-F29</f>
-        <v>19.940596599999992</v>
-      </c>
-      <c r="Y31">
-        <f>D31-D29</f>
-        <v>-0.77514599999994971</v>
-      </c>
-      <c r="Z31">
-        <f>ABS(Y31)/X31</f>
-        <v>3.8872758701710558E-2</v>
+        <v>176</v>
+      </c>
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-0.33046921299999998</v>
+        <v>-0.33030731299999999</v>
       </c>
       <c r="B32">
-        <v>-78.202250989999996</v>
+        <v>-78.202195029999999</v>
       </c>
       <c r="C32">
-        <v>4073.2315250000001</v>
+        <v>4074.1683619999999</v>
       </c>
       <c r="D32">
-        <v>4073.1472170000002</v>
+        <v>1658</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4922</v>
       </c>
       <c r="F32">
-        <v>244.6716424</v>
+        <v>225.19618750000001</v>
       </c>
       <c r="G32">
-        <v>200</v>
+        <v>4073.903564453125</v>
       </c>
       <c r="H32">
-        <v>1.5</v>
+        <v>180</v>
       </c>
       <c r="I32">
-        <v>41</v>
-      </c>
-      <c r="J32" s="1">
-        <v>44370</v>
-      </c>
-      <c r="K32">
-        <v>1.335</v>
-      </c>
-      <c r="L32">
-        <v>5068.8565470000003</v>
-      </c>
-      <c r="M32">
-        <v>3.4460000000000002</v>
-      </c>
-      <c r="N32">
-        <v>0.1113</v>
-      </c>
-      <c r="O32">
-        <v>6.7539999999999996</v>
-      </c>
-      <c r="P32">
-        <v>627.37040000000002</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>27</v>
-      </c>
-      <c r="R32" t="s">
-        <v>23</v>
-      </c>
-      <c r="S32" t="s">
-        <v>33</v>
-      </c>
-      <c r="T32">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>144</v>
+      </c>
+      <c r="U32">
         <v>10</v>
       </c>
-      <c r="U32" t="e">
-        <f>#REF!-F31</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V32" t="e">
-        <f>#REF!-D31</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W32" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="V32">
+        <f>F33-F30</f>
+        <v>19.940596599999992</v>
+      </c>
+      <c r="W32">
+        <f>G33-G30</f>
+        <v>-0.583251953125</v>
       </c>
       <c r="X32">
-        <f>F32-F30</f>
-        <v>19.475454899999988</v>
+        <f t="shared" si="1"/>
+        <v>2.9249473565149009E-2</v>
       </c>
       <c r="Y32">
-        <f>D32-D30</f>
-        <v>-0.82299799999964307</v>
+        <f>F32-F28</f>
+        <v>19.940596600000021</v>
       </c>
       <c r="Z32">
-        <f>ABS(Y32)/X32</f>
-        <v>4.2258217033977655E-2</v>
+        <f>G32-G28</f>
+        <v>-0.601318359375</v>
       </c>
       <c r="AA32">
-        <v>1.4984999999999999</v>
+        <f>ABS(Z32)/Y32</f>
+        <v>3.0155484885291715E-2</v>
       </c>
       <c r="AB32">
         <v>2.4800000000000001E-4</v>
       </c>
-      <c r="AC32">
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-0.33039551299999997</v>
+      </c>
+      <c r="B33">
+        <v>-78.202208720000002</v>
+      </c>
+      <c r="C33">
+        <v>4073.2208500000002</v>
+      </c>
+      <c r="D33">
+        <v>1661</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4949000000000001</v>
+      </c>
+      <c r="F33">
+        <v>235.1664858</v>
+      </c>
+      <c r="G33">
+        <v>4073.573486328125</v>
+      </c>
+      <c r="H33">
+        <v>190</v>
+      </c>
+      <c r="I33">
+        <v>5.5</v>
+      </c>
+      <c r="J33">
+        <v>40</v>
+      </c>
+      <c r="T33" t="s">
+        <v>32</v>
+      </c>
+      <c r="U33">
+        <v>10</v>
+      </c>
+      <c r="V33">
+        <f t="shared" ref="V33" si="2">F34-F32</f>
+        <v>19.475454899999988</v>
+      </c>
+      <c r="W33">
+        <f>G34-G32</f>
+        <v>-0.607177734375</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="1"/>
+        <v>3.1176562370052799E-2</v>
+      </c>
+      <c r="Y33">
+        <f>F33-F30</f>
+        <v>19.940596599999992</v>
+      </c>
+      <c r="Z33">
+        <f>G33-G30</f>
+        <v>-0.583251953125</v>
+      </c>
+      <c r="AA33">
+        <f>ABS(Z33)/Y33</f>
+        <v>2.9249473565149009E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-0.33046921299999998</v>
+      </c>
+      <c r="B34">
+        <v>-78.202250989999996</v>
+      </c>
+      <c r="C34">
+        <v>4073.2315250000001</v>
+      </c>
+      <c r="D34">
+        <v>1663</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4967000000000001</v>
+      </c>
+      <c r="F34">
+        <v>244.6716424</v>
+      </c>
+      <c r="G34">
+        <v>4073.29638671875</v>
+      </c>
+      <c r="H34">
+        <v>200</v>
+      </c>
+      <c r="I34">
+        <v>1.5</v>
+      </c>
+      <c r="J34">
+        <v>41</v>
+      </c>
+      <c r="K34" s="1">
+        <v>44370</v>
+      </c>
+      <c r="L34">
+        <v>1.335</v>
+      </c>
+      <c r="M34">
+        <v>5068.8565470000003</v>
+      </c>
+      <c r="N34">
+        <v>3.4460000000000002</v>
+      </c>
+      <c r="O34">
+        <v>0.1113</v>
+      </c>
+      <c r="P34">
+        <v>6.7539999999999996</v>
+      </c>
+      <c r="Q34">
+        <v>627.37040000000002</v>
+      </c>
+      <c r="R34" t="s">
+        <v>27</v>
+      </c>
+      <c r="S34" t="s">
+        <v>23</v>
+      </c>
+      <c r="T34" t="s">
+        <v>33</v>
+      </c>
+      <c r="U34">
+        <v>10</v>
+      </c>
+      <c r="V34">
+        <f>F35-F33</f>
+        <v>-0.4948434000000077</v>
+      </c>
+      <c r="W34">
+        <f>G35-G33</f>
+        <v>-0.87280232812508984</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="1"/>
+        <v>-1.7637950271238865</v>
+      </c>
+      <c r="Y34">
+        <f>F34-F32</f>
+        <v>19.475454899999988</v>
+      </c>
+      <c r="Z34">
+        <f>G34-G32</f>
+        <v>-0.607177734375</v>
+      </c>
+      <c r="AA34">
+        <f>ABS(Z34)/Y34</f>
+        <v>3.1176562370052799E-2</v>
+      </c>
+      <c r="AB34">
+        <v>2.4800000000000001E-4</v>
+      </c>
+      <c r="AC34">
         <v>9.5492500000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f>F34-10</f>
+        <v>234.6716424</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4072.7006839999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>